<commit_message>
Final df ready to start slicing and dicing
</commit_message>
<xml_diff>
--- a/data/specifications.xlsx
+++ b/data/specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\rm-evaluation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304EBEFA-DAFC-4A8E-A37C-8E07BE331851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57801077-C1B2-495D-972A-35B3EE67ED5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="specifications" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>product</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>BR0010P850</t>
+  </si>
+  <si>
+    <t>YL0010C229</t>
   </si>
 </sst>
 </file>
@@ -896,18 +899,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1020,6 +1023,104 @@
       </c>
       <c r="D8">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>-0.5</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>-0.5</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>-0.5</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>95</v>
+      </c>
+      <c r="D12">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>-0.5</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>-0.5</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>-0.5</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>